<commit_message>
The formulation was updated. The main.py was updated too. New constraints were added.
</commit_message>
<xml_diff>
--- a/test_mip_procure/data/outputs/Output.xlsx
+++ b/test_mip_procure/data/outputs/Output.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="patas_pack" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="pet_gourmet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="pet_gourmet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="patas_pack" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,12 +452,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Demand</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Transferred Quantity</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Acquired Quantity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -476,16 +476,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
         <v>1810</v>
       </c>
-      <c r="E2" t="n">
-        <v>1710</v>
-      </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
         <v>2500</v>
@@ -507,7 +507,7 @@
         <v>2500</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
         <v>2500</v>
@@ -529,7 +529,7 @@
         <v>2500</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -542,16 +542,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="n">
         <v>1960</v>
       </c>
-      <c r="E5" t="n">
-        <v>1860</v>
-      </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -564,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
         <v>2500</v>
@@ -573,7 +573,7 @@
         <v>2500</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -586,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
         <v>2500</v>
@@ -595,7 +595,7 @@
         <v>2500</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -608,16 +608,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D8" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E8" t="n">
         <v>2410</v>
       </c>
-      <c r="E8" t="n">
-        <v>2360</v>
-      </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -630,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
         <v>3000</v>
@@ -639,7 +639,7 @@
         <v>3000</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -652,7 +652,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>3000</v>
@@ -661,7 +661,7 @@
         <v>3000</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -674,16 +674,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D11" t="n">
-        <v>810</v>
+        <v>1000</v>
       </c>
       <c r="E11" t="n">
-        <v>710</v>
+        <v>2310</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="12">
@@ -696,16 +696,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1510</v>
       </c>
       <c r="D12" t="n">
         <v>1500</v>
       </c>
       <c r="E12" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -718,7 +718,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
         <v>1500</v>
@@ -727,7 +727,7 @@
         <v>1500</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -740,16 +740,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E14" t="n">
         <v>810</v>
       </c>
-      <c r="E14" t="n">
-        <v>710</v>
-      </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -762,16 +762,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
         <v>1000</v>
       </c>
       <c r="E15" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="16">
@@ -784,16 +784,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1010</v>
       </c>
       <c r="D16" t="n">
         <v>1000</v>
       </c>
       <c r="E16" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -806,16 +806,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>50</v>
+        <v>2900</v>
       </c>
       <c r="D17" t="n">
-        <v>1960</v>
+        <v>2000</v>
       </c>
       <c r="E17" t="n">
-        <v>1910</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
     </row>
     <row r="18">
@@ -828,16 +828,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="D18" t="n">
         <v>2000</v>
       </c>
       <c r="E18" t="n">
-        <v>2000</v>
+        <v>1110</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -850,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19" t="n">
         <v>2000</v>
@@ -859,7 +859,7 @@
         <v>2000</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -899,12 +899,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Demand</t>
+          <t>Transferred Quantity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Transferred Quantity</t>
+          <t>Acquired Quantity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -923,16 +923,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>2000</v>
+        <v>1810</v>
       </c>
       <c r="E2" t="n">
-        <v>1810</v>
+        <v>1710</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>2500</v>
@@ -954,7 +954,7 @@
         <v>2500</v>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -967,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>2500</v>
@@ -976,7 +976,7 @@
         <v>2500</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -989,16 +989,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>2000</v>
+        <v>1960</v>
       </c>
       <c r="E5" t="n">
-        <v>1960</v>
+        <v>1860</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1011,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>2500</v>
@@ -1020,7 +1020,7 @@
         <v>2500</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1033,7 +1033,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>2500</v>
@@ -1042,7 +1042,7 @@
         <v>2500</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1055,16 +1055,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D8" t="n">
-        <v>2500</v>
+        <v>2410</v>
       </c>
       <c r="E8" t="n">
-        <v>2410</v>
+        <v>2360</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1077,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>3000</v>
@@ -1086,7 +1086,7 @@
         <v>3000</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1099,7 +1099,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>3000</v>
@@ -1108,7 +1108,7 @@
         <v>3000</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1121,16 +1121,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D11" t="n">
-        <v>1000</v>
+        <v>2310</v>
       </c>
       <c r="E11" t="n">
-        <v>810</v>
+        <v>2210</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1143,16 +1143,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1165,7 +1165,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>1500</v>
@@ -1174,7 +1174,7 @@
         <v>1500</v>
       </c>
       <c r="F13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1187,16 +1187,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D14" t="n">
-        <v>1000</v>
+        <v>810</v>
       </c>
       <c r="E14" t="n">
-        <v>810</v>
+        <v>710</v>
       </c>
       <c r="F14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1209,16 +1209,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E15" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1231,16 +1231,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1256,13 +1256,13 @@
         <v>50</v>
       </c>
       <c r="D17" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1960</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
@@ -1275,16 +1275,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D18" t="n">
-        <v>2000</v>
+        <v>1110</v>
       </c>
       <c r="E18" t="n">
-        <v>2000</v>
+        <v>1060</v>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1297,7 +1297,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>2000</v>
@@ -1306,7 +1306,7 @@
         <v>2000</v>
       </c>
       <c r="F19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactory of the main.py and schemas.py. New data types were added for tables "distribution" and "items_aging"
</commit_message>
<xml_diff>
--- a/test_mip_procure/data/outputs/Output.xlsx
+++ b/test_mip_procure/data/outputs/Output.xlsx
@@ -680,10 +680,10 @@
         <v>1000</v>
       </c>
       <c r="E11" t="n">
-        <v>2310</v>
+        <v>810</v>
       </c>
       <c r="F11" t="n">
-        <v>1510</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -696,16 +696,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>1510</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
         <v>1500</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="13">
@@ -718,13 +718,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>1510</v>
       </c>
       <c r="D13" t="n">
         <v>1500</v>
       </c>
       <c r="E13" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>10</v>
@@ -746,10 +746,10 @@
         <v>1000</v>
       </c>
       <c r="E14" t="n">
-        <v>810</v>
+        <v>1810</v>
       </c>
       <c r="F14" t="n">
-        <v>10</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="15">
@@ -762,16 +762,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>1010</v>
       </c>
       <c r="D15" t="n">
         <v>1000</v>
       </c>
       <c r="E15" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>1010</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -784,13 +784,13 @@
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>1010</v>
+        <v>10</v>
       </c>
       <c r="D16" t="n">
         <v>1000</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F16" t="n">
         <v>10</v>
@@ -1124,10 +1124,10 @@
         <v>100</v>
       </c>
       <c r="D11" t="n">
-        <v>2310</v>
+        <v>810</v>
       </c>
       <c r="E11" t="n">
-        <v>2210</v>
+        <v>710</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1146,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1168,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -1190,10 +1190,10 @@
         <v>100</v>
       </c>
       <c r="D14" t="n">
-        <v>810</v>
+        <v>1810</v>
       </c>
       <c r="E14" t="n">
-        <v>710</v>
+        <v>1710</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1212,10 +1212,10 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1234,10 +1234,10 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>

</xml_diff>